<commit_message>
update 23 sectors result
</commit_message>
<xml_diff>
--- a/Data/result_table.xlsx
+++ b/Data/result_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eviriyakovithya\Documents\GitHub\SNA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1104A2C-BE52-43E8-8980-46933CD6ACFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282A78CA-A4DF-449B-9A33-2DB6B20983ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{4ECFBFB7-7C12-4BEA-A6DE-A9218C1989A2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>405 industries </t>
   </si>
@@ -281,34 +281,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +628,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -657,98 +657,98 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>14</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>8</v>
+      <c r="E2" s="6">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8"/>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <v>98</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>37</v>
       </c>
-      <c r="E3" s="10">
-        <v>17</v>
+      <c r="E3" s="8">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>5</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>4</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>20</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>9</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="11"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>221</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>12</v>
       </c>
     </row>

</xml_diff>